<commit_message>
Allocation now based on minimizing number of containers used while respecting whether container is suitable for each plant (depth, capacity etc)
</commit_message>
<xml_diff>
--- a/data/raw/PlantMaster.xlsx
+++ b/data/raw/PlantMaster.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\1.1. Research\Planting space optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DD36AD-186C-4312-91D0-1EC1155CEC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B058F01D-B8EA-4E85-9792-E9FB27E9F280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="500" windowWidth="14400" windowHeight="8270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>name</t>
   </si>
@@ -51,16 +60,16 @@
     <t>Zucchini</t>
   </si>
   <si>
-    <t>space_needed</t>
-  </si>
-  <si>
-    <t>sun</t>
-  </si>
-  <si>
-    <t>full</t>
-  </si>
-  <si>
-    <t>partial</t>
+    <t>depth_needed</t>
+  </si>
+  <si>
+    <t>Cotton</t>
+  </si>
+  <si>
+    <t>capacity_needed</t>
+  </si>
+  <si>
+    <t>Passion Fruit</t>
   </si>
 </sst>
 </file>
@@ -381,17 +390,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -402,7 +412,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -410,10 +420,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -421,10 +431,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>45</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -434,8 +444,8 @@
       <c r="B4" s="1">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
+      <c r="C4" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -443,10 +453,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -454,10 +464,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -465,9 +475,9 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1">
         <v>10</v>
       </c>
     </row>
@@ -476,10 +486,32 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>60</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="C8" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>90</v>
+      </c>
+      <c r="C10" s="1">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>